<commit_message>
BioretentionBlues: Fix datum on pond
Changed the calculation of pressure head into the filter zone to set the datum to the bottom of the pond rather than the bottom of the filter zone, as that was causing a dependency on filter depth which didn't work with the design scenarios. Also finalized calibration with this new configuration and ran IDF curves
</commit_message>
<xml_diff>
--- a/inputfiles/params_Pine8th_1.xlsx
+++ b/inputfiles/params_Pine8th_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\SubsurfaceSinks\inputfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C92FC9-2F06-4380-BBA2-05C2E28DC4F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32D49500-F363-4862-B3F6-1241DFCE2AF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="14475" windowHeight="3780" xr2:uid="{DF45CC4F-1F30-4014-8BCA-4F35CD4112BF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="14472" windowHeight="3780" xr2:uid="{DF45CC4F-1F30-4014-8BCA-4F35CD4112BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -641,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -672,6 +672,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -992,17 +1002,17 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="J78" sqref="J78"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1954,8 +1964,8 @@
       <c r="A70" t="s">
         <v>101</v>
       </c>
-      <c r="B70" s="3">
-        <v>0.19768124000000001</v>
+      <c r="B70" s="15">
+        <v>0.20955119</v>
       </c>
       <c r="C70" t="s">
         <v>166</v>
@@ -1970,7 +1980,7 @@
       <c r="A71" t="s">
         <v>131</v>
       </c>
-      <c r="B71" s="11">
+      <c r="B71" s="16">
         <v>0.125</v>
       </c>
       <c r="C71" t="s">
@@ -1985,8 +1995,8 @@
       <c r="A72" t="s">
         <v>173</v>
       </c>
-      <c r="B72">
-        <v>0.19605502</v>
+      <c r="B72" s="14">
+        <v>0.16522809999999999</v>
       </c>
       <c r="C72" t="s">
         <v>174</v>
@@ -2000,7 +2010,7 @@
       <c r="A73" t="s">
         <v>85</v>
       </c>
-      <c r="B73" s="3">
+      <c r="B73" s="15">
         <v>10.000011539999999</v>
       </c>
       <c r="C73" t="s">
@@ -2013,7 +2023,7 @@
       <c r="A74" t="s">
         <v>7</v>
       </c>
-      <c r="B74" s="3">
+      <c r="B74" s="15">
         <v>0.19532010999999999</v>
       </c>
       <c r="C74" t="s">
@@ -2027,7 +2037,7 @@
       <c r="A75" t="s">
         <v>9</v>
       </c>
-      <c r="B75" s="12">
+      <c r="B75" s="17">
         <v>0.67638900000000002</v>
       </c>
       <c r="C75" t="s">
@@ -2053,7 +2063,7 @@
       <c r="A76" t="s">
         <v>132</v>
       </c>
-      <c r="B76" s="14">
+      <c r="B76" s="18">
         <v>100</v>
       </c>
       <c r="C76" t="s">
@@ -2064,8 +2074,8 @@
       <c r="A77" t="s">
         <v>154</v>
       </c>
-      <c r="B77" s="11">
-        <v>2.89863953E-4</v>
+      <c r="B77" s="16">
+        <v>2.8152436700000001E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>